<commit_message>
Adding choice filtering for selects
</commit_message>
<xml_diff>
--- a/form-files/imnci/IMNCI_up_to_2mo.xlsx
+++ b/form-files/imnci/IMNCI_up_to_2mo.xlsx
@@ -241,9 +241,6 @@
     <t xml:space="preserve">If breastfeeding less than 8 times  in 24 hours, advise to increase frequency of feeding. </t>
   </si>
   <si>
-    <t>possible_serious_bacterial_infection_agree</t>
-  </si>
-  <si>
     <t>Female</t>
   </si>
   <si>
@@ -275,6 +272,9 @@
   </si>
   <si>
     <t>goto_if lbi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_months </t>
   </si>
   <si>
     <t xml:space="preserve"> PROBLEMS:
@@ -497,9 +497,6 @@
     <t>refer_urgently_to_hospital_w_ORS</t>
   </si>
   <si>
-    <t>monthsAge</t>
-  </si>
-  <si>
     <t xml:space="preserve">ASK: Does the mother have pain while breastfeeding? </t>
   </si>
   <si>
@@ -606,12 +603,12 @@
     <t>some keeping infant warm instructions are more specific</t>
   </si>
   <si>
+    <t>Value must be yes, for now.</t>
+  </si>
+  <si>
     <t>use_to_feed</t>
   </si>
   <si>
-    <t>Value must be yes, for now.</t>
-  </si>
-  <si>
     <t>goto_if dehydration</t>
   </si>
   <si>
@@ -631,6 +628,9 @@
   </si>
   <si>
     <t>label severe_dysentery</t>
+  </si>
+  <si>
+    <t>context.age_months &lt; V('age_months')</t>
   </si>
   <si>
     <t>observe_breastfeed</t>
@@ -816,6 +816,9 @@
   </si>
   <si>
     <t>visible_areola</t>
+  </si>
+  <si>
+    <t>choiceFilter</t>
   </si>
   <si>
     <t>selected({{skin_pustules}}, 'yes')</t>
@@ -1027,9 +1030,6 @@
   </si>
   <si>
     <t>Is there any indication for urgent referral?</t>
-  </si>
-  <si>
-    <t>relevant</t>
   </si>
   <si>
     <t>Chin touching breast</t>
@@ -1586,10 +1586,10 @@
   <sheetData>
     <row r="1" ht="28.5">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>104</v>
@@ -1604,13 +1604,13 @@
         <v>321</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>268</v>
-      </c>
       <c r="I1" s="2" t="s">
-        <v>309</v>
+        <v>248</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>211</v>
@@ -1619,10 +1619,10 @@
         <v>113</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" ht="128.25">
@@ -1630,11 +1630,11 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>127</v>
@@ -1648,7 +1648,7 @@
         <v>134</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" ht="16.5" customHeight="1">
@@ -1670,14 +1670,14 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="3" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" ht="57">
       <c r="A5" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>55</v>
@@ -1728,7 +1728,7 @@
         <v>39</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>217</v>
@@ -1744,7 +1744,7 @@
     <row r="8" ht="16.5" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1786,10 +1786,10 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="2"/>
@@ -1806,7 +1806,7 @@
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>45</v>
@@ -1831,14 +1831,14 @@
     <row r="13" ht="16.5" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
         <v>331</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1866,14 +1866,14 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>142</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="H15" s="4" t="b">
         <v>1</v>
@@ -1891,7 +1891,7 @@
         <v>32</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H16" s="4" t="b">
         <v>1</v>
@@ -1906,10 +1906,10 @@
         <v>116</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H17" s="4" t="b">
         <v>1</v>
@@ -1924,10 +1924,10 @@
         <v>136</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H18" s="4" t="b">
         <v>1</v>
@@ -1936,13 +1936,13 @@
     <row r="19" ht="16.5" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>90</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="F19" s="3"/>
       <c r="H19" s="4" t="b">
@@ -1989,7 +1989,7 @@
         <v>326</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F22" s="3"/>
     </row>
@@ -2012,7 +2012,7 @@
     <row r="24" ht="16.5" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -2021,10 +2021,10 @@
     <row r="25" ht="16.5" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>59</v>
@@ -2037,13 +2037,13 @@
     <row r="26" ht="16.5" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>243</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F26" s="3"/>
       <c r="H26" s="4" t="b">
@@ -2053,13 +2053,13 @@
     <row r="27" ht="16.5" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="F27" s="3"/>
       <c r="H27" s="4" t="b">
@@ -2068,13 +2068,13 @@
     </row>
     <row r="28" ht="242.25">
       <c r="A28" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>117</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -2127,7 +2127,7 @@
         <v>117</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -2144,7 +2144,7 @@
         <v>117</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -2161,7 +2161,7 @@
         <v>117</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -2212,7 +2212,7 @@
         <v>117</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -2225,10 +2225,10 @@
     </row>
     <row r="37" ht="114">
       <c r="A37" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>135</v>
@@ -2248,10 +2248,10 @@
     </row>
     <row r="38" ht="42.75">
       <c r="A38" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>42</v>
@@ -2272,7 +2272,7 @@
     <row r="39" ht="57">
       <c r="A39" s="1"/>
       <c r="B39" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>105</v>
@@ -2289,10 +2289,10 @@
     <row r="40" ht="42.75">
       <c r="A40" s="1"/>
       <c r="B40" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -2343,14 +2343,11 @@
       <c r="B44" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="D44" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="E44" s="4" t="s">
         <v>145</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="45" ht="199.5">
@@ -2389,7 +2386,7 @@
         <v>140</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G47" s="2"/>
       <c r="H47" s="4" t="b">
@@ -2405,7 +2402,7 @@
         <v>94</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G48" s="2"/>
       <c r="H48" s="4" t="b">
@@ -2431,7 +2428,7 @@
     <row r="50" ht="16.5" customHeight="1">
       <c r="A50" s="1"/>
       <c r="B50" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2" t="s">
@@ -2439,9 +2436,6 @@
       </c>
       <c r="E50" s="2"/>
       <c r="G50" s="2"/>
-      <c r="H50" s="4" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="51" ht="16.5" customHeight="1">
       <c r="A51" s="1"/>
@@ -2473,7 +2467,7 @@
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G53" s="2"/>
     </row>
@@ -2487,10 +2481,10 @@
         <v>13</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G54" s="2"/>
     </row>
@@ -2521,7 +2515,7 @@
         <v>99</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="G56" s="2"/>
       <c r="H56" s="4" t="b">
@@ -2537,7 +2531,7 @@
         <v>23</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G57" s="2"/>
       <c r="H57" s="4" t="b">
@@ -2547,11 +2541,11 @@
     <row r="58" ht="16.5" customHeight="1">
       <c r="A58" s="1"/>
       <c r="B58" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E58" s="2"/>
       <c r="G58" s="2"/>
@@ -2582,13 +2576,13 @@
     <row r="61" ht="256.5">
       <c r="A61" s="1"/>
       <c r="B61" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>24</v>
@@ -2641,7 +2635,7 @@
     <row r="64" ht="16.5" customHeight="1">
       <c r="A64" s="1"/>
       <c r="B64" s="5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E64" s="2"/>
       <c r="H64" s="4" t="b">
@@ -2656,13 +2650,13 @@
     <row r="65" ht="16.5" customHeight="1">
       <c r="A65" s="1"/>
       <c r="B65" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H65" s="4" t="b">
         <v>1</v>
@@ -2676,10 +2670,10 @@
     <row r="66" ht="16.5" customHeight="1">
       <c r="A66" s="1"/>
       <c r="B66" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
@@ -2720,7 +2714,7 @@
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H68" s="4" t="b">
         <v>1</v>
@@ -2734,7 +2728,7 @@
     <row r="69" ht="57">
       <c r="A69" s="1"/>
       <c r="B69" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>328</v>
@@ -2756,10 +2750,10 @@
     <row r="70" ht="16.5" customHeight="1">
       <c r="A70" s="1"/>
       <c r="B70" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>111</v>
@@ -2776,7 +2770,7 @@
     <row r="71" ht="28.5">
       <c r="A71" s="1"/>
       <c r="B71" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>238</v>
@@ -2804,10 +2798,10 @@
     <row r="73" ht="42.75">
       <c r="A73" s="1"/>
       <c r="B73" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>234</v>
@@ -2846,7 +2840,7 @@
     <row r="75" ht="16.5" customHeight="1">
       <c r="A75" s="1"/>
       <c r="B75" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>86</v>
@@ -2858,7 +2852,7 @@
     <row r="76" ht="16.5" customHeight="1">
       <c r="A76" s="1"/>
       <c r="B76" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>44</v>
@@ -2906,7 +2900,7 @@
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F80" s="4" t="s">
         <v>4</v>
@@ -2918,7 +2912,7 @@
     </row>
     <row r="81" ht="185.25">
       <c r="A81" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>221</v>
@@ -3001,7 +2995,7 @@
     <row r="86" ht="16.5" customHeight="1">
       <c r="A86" s="1"/>
       <c r="B86" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="87" ht="42.75">
@@ -3016,7 +3010,7 @@
     <row r="88" ht="16.5" customHeight="1">
       <c r="A88" s="1"/>
       <c r="B88" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
@@ -3034,7 +3028,7 @@
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
       <c r="E89" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F89" s="4" t="s">
         <v>139</v>
@@ -3072,7 +3066,7 @@
     <row r="92" ht="42.75">
       <c r="A92" s="1"/>
       <c r="B92" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H92" s="4" t="b">
         <v>1</v>
@@ -3110,7 +3104,7 @@
         <v>123</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E95" s="4" t="s">
         <v>21</v>
@@ -3125,7 +3119,7 @@
         <v>12</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="97" ht="57">
@@ -3142,7 +3136,7 @@
     </row>
     <row r="98" ht="71.25">
       <c r="A98" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>123</v>
@@ -3160,7 +3154,7 @@
     <row r="99" ht="16.5" customHeight="1">
       <c r="A99" s="1"/>
       <c r="B99" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="100" ht="42.75">
@@ -3178,7 +3172,7 @@
     <row r="102" ht="42.75">
       <c r="A102" s="1"/>
       <c r="B102" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H102" s="4" t="b">
         <v>1</v>
@@ -3187,10 +3181,10 @@
     <row r="103" ht="42.75">
       <c r="A103" s="1"/>
       <c r="B103" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E103" s="4" t="s">
         <v>65</v>
@@ -3202,7 +3196,7 @@
     <row r="104" ht="42.75">
       <c r="A104" s="1"/>
       <c r="B104" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D104" s="4" t="s">
         <v>239</v>
@@ -3220,7 +3214,7 @@
         <v>55</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D105" s="4" t="s">
         <v>128</v>
@@ -3232,7 +3226,7 @@
     <row r="106" ht="114">
       <c r="A106" s="1"/>
       <c r="B106" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D106" s="4" t="s">
         <v>88</v>
@@ -3263,7 +3257,7 @@
         <v>57</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D108" s="4" t="s">
         <v>184</v>
@@ -3277,13 +3271,13 @@
         <v>31</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D109" s="4" t="s">
         <v>96</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H109" s="4" t="b">
         <v>1</v>
@@ -3309,7 +3303,7 @@
         <v>193</v>
       </c>
       <c r="E111" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H111" s="4" t="b">
         <v>1</v>
@@ -3318,10 +3312,10 @@
     <row r="112" ht="42.75">
       <c r="A112" s="1"/>
       <c r="B112" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E112" s="4" t="s">
         <v>312</v>
@@ -3332,7 +3326,7 @@
         <v>108</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C113" s="2"/>
       <c r="D113" s="2" t="s">
@@ -3361,7 +3355,7 @@
         <v>38</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="F114" s="3" t="s">
         <v>316</v>
@@ -3379,7 +3373,7 @@
     <row r="115" ht="16.5" customHeight="1">
       <c r="A115" s="1"/>
       <c r="B115" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
@@ -3395,11 +3389,11 @@
     <row r="116" ht="16.5" customHeight="1">
       <c r="A116" s="1"/>
       <c r="B116" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C116" s="2"/>
       <c r="D116" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>313</v>
@@ -3418,13 +3412,13 @@
     <row r="117" ht="85.5">
       <c r="A117" s="1"/>
       <c r="B117" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E117" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H117" s="4" t="b">
         <v>1</v>
@@ -3436,13 +3430,13 @@
         <v>207</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E118" s="4" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="119" ht="71.25">
@@ -3453,7 +3447,7 @@
         <v>207</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D119" s="4" t="s">
         <v>216</v>
@@ -3488,7 +3482,7 @@
     <row r="121" ht="16.5" customHeight="1">
       <c r="A121" s="1"/>
       <c r="B121" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>203</v>
@@ -3529,7 +3523,7 @@
       <c r="C123" s="2"/>
       <c r="D123" s="2"/>
       <c r="E123" s="4" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F123" s="3" t="s">
         <v>46</v>
@@ -3570,10 +3564,10 @@
       </c>
       <c r="C125" s="2"/>
       <c r="D125" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G125" s="2"/>
       <c r="H125" s="4" t="b">
@@ -3588,7 +3582,7 @@
     <row r="126" ht="16.5" customHeight="1">
       <c r="A126" s="1"/>
       <c r="B126" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C126" s="2"/>
       <c r="D126" s="2"/>
@@ -3664,7 +3658,7 @@
         <v>112</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G130" s="2"/>
       <c r="H130" s="4" t="b">
@@ -3829,7 +3823,7 @@
         <v>23</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G138" s="2"/>
       <c r="H138" s="4" t="b">
@@ -3844,7 +3838,7 @@
     <row r="139" ht="16.5" customHeight="1">
       <c r="A139" s="1"/>
       <c r="B139" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C139" s="2"/>
       <c r="D139" s="2"/>
@@ -3875,7 +3869,7 @@
     <row r="141" ht="16.5" customHeight="1">
       <c r="A141" s="1"/>
       <c r="B141" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C141" s="2"/>
       <c r="D141" s="2"/>
@@ -3911,7 +3905,7 @@
       <c r="C143" s="2"/>
       <c r="D143" s="2"/>
       <c r="E143" s="4" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F143" s="3" t="s">
         <v>229</v>
@@ -3930,10 +3924,10 @@
       </c>
       <c r="C144" s="2"/>
       <c r="D144" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G144" s="2"/>
       <c r="H144" s="4" t="b">
@@ -3955,7 +3949,7 @@
         <v>12</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="G145" s="2"/>
       <c r="H145" s="4" t="b">
@@ -3970,7 +3964,7 @@
     <row r="146" ht="16.5" customHeight="1">
       <c r="A146" s="1"/>
       <c r="B146" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C146" s="2"/>
       <c r="D146" s="2"/>
@@ -4037,18 +4031,20 @@
         <v>80</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C150" s="2"/>
       <c r="D150" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="F150" s="3"/>
       <c r="G150" s="2"/>
-      <c r="I150" s="4"/>
+      <c r="I150" s="4" t="s">
+        <v>192</v>
+      </c>
       <c r="J150" s="4"/>
       <c r="K150" s="4"/>
       <c r="L150" s="4"/>
@@ -4277,7 +4273,7 @@
   <sheetData>
     <row r="1" ht="14.25">
       <c r="A1" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>133</v>
@@ -4286,7 +4282,7 @@
         <v>110</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>149</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" ht="14.25">
@@ -4297,7 +4293,7 @@
         <v>63</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" ht="14.25">
@@ -4305,7 +4301,7 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>233</v>
@@ -4332,7 +4328,7 @@
         <v>195</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>231</v>
@@ -4345,10 +4341,10 @@
     </row>
     <row r="8" ht="14.25">
       <c r="A8" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>58</v>
@@ -4356,10 +4352,10 @@
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>223</v>
@@ -4378,7 +4374,7 @@
         <v>230</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" ht="14.25">
@@ -4386,10 +4382,10 @@
         <v>122</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" ht="14.25">
@@ -4409,7 +4405,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" ht="14.25">
@@ -4438,18 +4434,18 @@
     <row r="19" ht="12.75" customHeight="1"/>
     <row r="20" ht="42.75">
       <c r="A20" s="4" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="21" ht="28.5">
       <c r="A21" s="4" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>317</v>
@@ -4460,7 +4456,7 @@
     </row>
     <row r="22" ht="28.5">
       <c r="A22" s="4" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>84</v>
@@ -4480,10 +4476,10 @@
         <v>38</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="26" ht="28.5">
@@ -4505,7 +4501,7 @@
         <v>213</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="28" ht="12.75" customHeight="1"/>
@@ -4529,7 +4525,7 @@
         <v>3</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>1</v>
@@ -4543,10 +4539,10 @@
         <v>3</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D32" s="4" t="n">
         <v>1.5</v>
@@ -4570,7 +4566,7 @@
     <row r="35" ht="12.75" customHeight="1"/>
     <row r="36" ht="14.25">
       <c r="A36" s="4" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>225</v>
@@ -4581,7 +4577,7 @@
     </row>
     <row r="37" ht="14.25">
       <c r="A37" s="4" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>332</v>
@@ -4592,7 +4588,7 @@
     </row>
     <row r="38" ht="14.25">
       <c r="A38" s="4" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>324</v>
@@ -4608,7 +4604,7 @@
         <v>54</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>310</v>
@@ -4619,10 +4615,10 @@
         <v>54</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="43" ht="42.75">
@@ -4681,7 +4677,7 @@
         <v>129</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" ht="14.25">
@@ -4689,12 +4685,12 @@
         <v>89</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B3" s="4" t="n">
         <v>1.0</v>
@@ -4702,7 +4698,7 @@
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>6</v>

</xml_diff>